<commit_message>
refactoring in subdirectories, launch.json, layout automation for surveying.
</commit_message>
<xml_diff>
--- a/data/SURVEYING.xlsx
+++ b/data/SURVEYING.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q21"/>
+  <dimension ref="A1:X21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -519,6 +519,41 @@
           <t>UBI</t>
         </is>
       </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>LTD</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>LTM</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>LTS</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>LND</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>LNM</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>LNS</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -557,11 +592,38 @@
           <t>EGM08D595</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr"/>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>100.0516</t>
+        </is>
+      </c>
       <c r="N2" t="inlineStr"/>
       <c r="O2" t="inlineStr"/>
       <c r="P2" t="inlineStr"/>
       <c r="Q2" t="inlineStr"/>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>48.9676</t>
+        </is>
+      </c>
+      <c r="S2" t="n">
+        <v>41</v>
+      </c>
+      <c r="T2" t="n">
+        <v>20</v>
+      </c>
+      <c r="U2" t="n">
+        <v>26.7106571498374</v>
+      </c>
+      <c r="V2" t="n">
+        <v>2</v>
+      </c>
+      <c r="W2" t="n">
+        <v>9</v>
+      </c>
+      <c r="X2" t="n">
+        <v>52.46680573167545</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -602,13 +664,36 @@
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>100.0516</t>
+          <t>51.8971</t>
         </is>
       </c>
       <c r="N3" t="inlineStr"/>
       <c r="O3" t="inlineStr"/>
       <c r="P3" t="inlineStr"/>
       <c r="Q3" t="inlineStr"/>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>48.9561</t>
+        </is>
+      </c>
+      <c r="S3" t="n">
+        <v>41</v>
+      </c>
+      <c r="T3" t="n">
+        <v>19</v>
+      </c>
+      <c r="U3" t="n">
+        <v>35.70145709855183</v>
+      </c>
+      <c r="V3" t="n">
+        <v>2</v>
+      </c>
+      <c r="W3" t="n">
+        <v>8</v>
+      </c>
+      <c r="X3" t="n">
+        <v>32.11599954935174</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -649,13 +734,36 @@
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>51.8971</t>
+          <t>52.3443</t>
         </is>
       </c>
       <c r="N4" t="inlineStr"/>
       <c r="O4" t="inlineStr"/>
       <c r="P4" t="inlineStr"/>
       <c r="Q4" t="inlineStr"/>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>48.9543</t>
+        </is>
+      </c>
+      <c r="S4" t="n">
+        <v>41</v>
+      </c>
+      <c r="T4" t="n">
+        <v>19</v>
+      </c>
+      <c r="U4" t="n">
+        <v>33.16839982050851</v>
+      </c>
+      <c r="V4" t="n">
+        <v>2</v>
+      </c>
+      <c r="W4" t="n">
+        <v>8</v>
+      </c>
+      <c r="X4" t="n">
+        <v>31.46404049253391</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -696,13 +804,36 @@
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>52.3443</t>
+          <t>51.9766</t>
         </is>
       </c>
       <c r="N5" t="inlineStr"/>
       <c r="O5" t="inlineStr"/>
       <c r="P5" t="inlineStr"/>
       <c r="Q5" t="inlineStr"/>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>48.9406</t>
+        </is>
+      </c>
+      <c r="S5" t="n">
+        <v>41</v>
+      </c>
+      <c r="T5" t="n">
+        <v>19</v>
+      </c>
+      <c r="U5" t="n">
+        <v>25.11875552282334</v>
+      </c>
+      <c r="V5" t="n">
+        <v>2</v>
+      </c>
+      <c r="W5" t="n">
+        <v>8</v>
+      </c>
+      <c r="X5" t="n">
+        <v>48.65540848184445</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -743,13 +874,36 @@
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>51.9766</t>
+          <t>51.9616</t>
         </is>
       </c>
       <c r="N6" t="inlineStr"/>
       <c r="O6" t="inlineStr"/>
       <c r="P6" t="inlineStr"/>
       <c r="Q6" t="inlineStr"/>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>48.9406</t>
+        </is>
+      </c>
+      <c r="S6" t="n">
+        <v>41</v>
+      </c>
+      <c r="T6" t="n">
+        <v>19</v>
+      </c>
+      <c r="U6" t="n">
+        <v>25.11882324071223</v>
+      </c>
+      <c r="V6" t="n">
+        <v>2</v>
+      </c>
+      <c r="W6" t="n">
+        <v>8</v>
+      </c>
+      <c r="X6" t="n">
+        <v>48.65579474154387</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -790,13 +944,36 @@
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>51.9616</t>
+          <t>51.9184</t>
         </is>
       </c>
       <c r="N7" t="inlineStr"/>
       <c r="O7" t="inlineStr"/>
       <c r="P7" t="inlineStr"/>
       <c r="Q7" t="inlineStr"/>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>48.9354</t>
+        </is>
+      </c>
+      <c r="S7" t="n">
+        <v>41</v>
+      </c>
+      <c r="T7" t="n">
+        <v>19</v>
+      </c>
+      <c r="U7" t="n">
+        <v>17.98430469970413</v>
+      </c>
+      <c r="V7" t="n">
+        <v>2</v>
+      </c>
+      <c r="W7" t="n">
+        <v>8</v>
+      </c>
+      <c r="X7" t="n">
+        <v>46.76944868692495</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -837,13 +1014,36 @@
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>51.9184</t>
+          <t>51.9414</t>
         </is>
       </c>
       <c r="N8" t="inlineStr"/>
       <c r="O8" t="inlineStr"/>
       <c r="P8" t="inlineStr"/>
       <c r="Q8" t="inlineStr"/>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>48.9354</t>
+        </is>
+      </c>
+      <c r="S8" t="n">
+        <v>41</v>
+      </c>
+      <c r="T8" t="n">
+        <v>19</v>
+      </c>
+      <c r="U8" t="n">
+        <v>17.98511881471313</v>
+      </c>
+      <c r="V8" t="n">
+        <v>2</v>
+      </c>
+      <c r="W8" t="n">
+        <v>8</v>
+      </c>
+      <c r="X8" t="n">
+        <v>46.76991122247561</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -884,13 +1084,36 @@
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>51.9414</t>
+          <t>52.4805</t>
         </is>
       </c>
       <c r="N9" t="inlineStr"/>
       <c r="O9" t="inlineStr"/>
       <c r="P9" t="inlineStr"/>
       <c r="Q9" t="inlineStr"/>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>48.9475</t>
+        </is>
+      </c>
+      <c r="S9" t="n">
+        <v>41</v>
+      </c>
+      <c r="T9" t="n">
+        <v>19</v>
+      </c>
+      <c r="U9" t="n">
+        <v>20.63749414482231</v>
+      </c>
+      <c r="V9" t="n">
+        <v>2</v>
+      </c>
+      <c r="W9" t="n">
+        <v>8</v>
+      </c>
+      <c r="X9" t="n">
+        <v>22.82304878752715</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -931,13 +1154,36 @@
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>52.4805</t>
+          <t>52.4905</t>
         </is>
       </c>
       <c r="N10" t="inlineStr"/>
       <c r="O10" t="inlineStr"/>
       <c r="P10" t="inlineStr"/>
       <c r="Q10" t="inlineStr"/>
+      <c r="R10" t="inlineStr">
+        <is>
+          <t>48.9475</t>
+        </is>
+      </c>
+      <c r="S10" t="n">
+        <v>41</v>
+      </c>
+      <c r="T10" t="n">
+        <v>19</v>
+      </c>
+      <c r="U10" t="n">
+        <v>20.63739655082543</v>
+      </c>
+      <c r="V10" t="n">
+        <v>2</v>
+      </c>
+      <c r="W10" t="n">
+        <v>8</v>
+      </c>
+      <c r="X10" t="n">
+        <v>22.82300705611043</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -978,13 +1224,36 @@
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>52.4905</t>
+          <t>52.4765</t>
         </is>
       </c>
       <c r="N11" t="inlineStr"/>
       <c r="O11" t="inlineStr"/>
       <c r="P11" t="inlineStr"/>
       <c r="Q11" t="inlineStr"/>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>48.9635</t>
+        </is>
+      </c>
+      <c r="S11" t="n">
+        <v>41</v>
+      </c>
+      <c r="T11" t="n">
+        <v>19</v>
+      </c>
+      <c r="U11" t="n">
+        <v>21.64800740920953</v>
+      </c>
+      <c r="V11" t="n">
+        <v>2</v>
+      </c>
+      <c r="W11" t="n">
+        <v>7</v>
+      </c>
+      <c r="X11" t="n">
+        <v>46.99888501452591</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1025,13 +1294,36 @@
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>52.4765</t>
+          <t>52.5015</t>
         </is>
       </c>
       <c r="N12" t="inlineStr"/>
       <c r="O12" t="inlineStr"/>
       <c r="P12" t="inlineStr"/>
       <c r="Q12" t="inlineStr"/>
+      <c r="R12" t="inlineStr">
+        <is>
+          <t>48.9635</t>
+        </is>
+      </c>
+      <c r="S12" t="n">
+        <v>41</v>
+      </c>
+      <c r="T12" t="n">
+        <v>19</v>
+      </c>
+      <c r="U12" t="n">
+        <v>21.64816757838025</v>
+      </c>
+      <c r="V12" t="n">
+        <v>2</v>
+      </c>
+      <c r="W12" t="n">
+        <v>7</v>
+      </c>
+      <c r="X12" t="n">
+        <v>46.99862479207273</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1072,13 +1364,36 @@
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>52.5015</t>
+          <t>52.4975</t>
         </is>
       </c>
       <c r="N13" t="inlineStr"/>
       <c r="O13" t="inlineStr"/>
       <c r="P13" t="inlineStr"/>
       <c r="Q13" t="inlineStr"/>
+      <c r="R13" t="inlineStr">
+        <is>
+          <t>48.9635</t>
+        </is>
+      </c>
+      <c r="S13" t="n">
+        <v>41</v>
+      </c>
+      <c r="T13" t="n">
+        <v>19</v>
+      </c>
+      <c r="U13" t="n">
+        <v>21.64814003256822</v>
+      </c>
+      <c r="V13" t="n">
+        <v>2</v>
+      </c>
+      <c r="W13" t="n">
+        <v>7</v>
+      </c>
+      <c r="X13" t="n">
+        <v>46.99927038701023</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1119,13 +1434,36 @@
       </c>
       <c r="M14" t="inlineStr">
         <is>
-          <t>52.4975</t>
+          <t>53.3178</t>
         </is>
       </c>
       <c r="N14" t="inlineStr"/>
       <c r="O14" t="inlineStr"/>
       <c r="P14" t="inlineStr"/>
       <c r="Q14" t="inlineStr"/>
+      <c r="R14" t="inlineStr">
+        <is>
+          <t>48.9598</t>
+        </is>
+      </c>
+      <c r="S14" t="n">
+        <v>41</v>
+      </c>
+      <c r="T14" t="n">
+        <v>19</v>
+      </c>
+      <c r="U14" t="n">
+        <v>21.38552922561189</v>
+      </c>
+      <c r="V14" t="n">
+        <v>2</v>
+      </c>
+      <c r="W14" t="n">
+        <v>7</v>
+      </c>
+      <c r="X14" t="n">
+        <v>54.66617734017387</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1166,13 +1504,36 @@
       </c>
       <c r="M15" t="inlineStr">
         <is>
-          <t>53.3178</t>
+          <t>53.3108</t>
         </is>
       </c>
       <c r="N15" t="inlineStr"/>
       <c r="O15" t="inlineStr"/>
       <c r="P15" t="inlineStr"/>
       <c r="Q15" t="inlineStr"/>
+      <c r="R15" t="inlineStr">
+        <is>
+          <t>48.9598</t>
+        </is>
+      </c>
+      <c r="S15" t="n">
+        <v>41</v>
+      </c>
+      <c r="T15" t="n">
+        <v>19</v>
+      </c>
+      <c r="U15" t="n">
+        <v>21.38562682239694</v>
+      </c>
+      <c r="V15" t="n">
+        <v>2</v>
+      </c>
+      <c r="W15" t="n">
+        <v>7</v>
+      </c>
+      <c r="X15" t="n">
+        <v>54.66621906000306</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1213,13 +1574,36 @@
       </c>
       <c r="M16" t="inlineStr">
         <is>
-          <t>53.3108</t>
+          <t>52.9321</t>
         </is>
       </c>
       <c r="N16" t="inlineStr"/>
       <c r="O16" t="inlineStr"/>
       <c r="P16" t="inlineStr"/>
       <c r="Q16" t="inlineStr"/>
+      <c r="R16" t="inlineStr">
+        <is>
+          <t>48.9521</t>
+        </is>
+      </c>
+      <c r="S16" t="n">
+        <v>41</v>
+      </c>
+      <c r="T16" t="n">
+        <v>19</v>
+      </c>
+      <c r="U16" t="n">
+        <v>19.61109632877708</v>
+      </c>
+      <c r="V16" t="n">
+        <v>2</v>
+      </c>
+      <c r="W16" t="n">
+        <v>8</v>
+      </c>
+      <c r="X16" t="n">
+        <v>9.614466331483555</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1260,13 +1644,36 @@
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>52.9321</t>
+          <t>52.5073</t>
         </is>
       </c>
       <c r="N17" t="inlineStr"/>
       <c r="O17" t="inlineStr"/>
       <c r="P17" t="inlineStr"/>
       <c r="Q17" t="inlineStr"/>
+      <c r="R17" t="inlineStr">
+        <is>
+          <t>48.9513</t>
+        </is>
+      </c>
+      <c r="S17" t="n">
+        <v>41</v>
+      </c>
+      <c r="T17" t="n">
+        <v>19</v>
+      </c>
+      <c r="U17" t="n">
+        <v>20.44438711033138</v>
+      </c>
+      <c r="V17" t="n">
+        <v>2</v>
+      </c>
+      <c r="W17" t="n">
+        <v>8</v>
+      </c>
+      <c r="X17" t="n">
+        <v>13.19826761875039</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1307,13 +1714,36 @@
       </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>52.5073</t>
+          <t>52.5698</t>
         </is>
       </c>
       <c r="N18" t="inlineStr"/>
       <c r="O18" t="inlineStr"/>
       <c r="P18" t="inlineStr"/>
       <c r="Q18" t="inlineStr"/>
+      <c r="R18" t="inlineStr">
+        <is>
+          <t>48.9568</t>
+        </is>
+      </c>
+      <c r="S18" t="n">
+        <v>41</v>
+      </c>
+      <c r="T18" t="n">
+        <v>19</v>
+      </c>
+      <c r="U18" t="n">
+        <v>29.30799650146184</v>
+      </c>
+      <c r="V18" t="n">
+        <v>2</v>
+      </c>
+      <c r="W18" t="n">
+        <v>8</v>
+      </c>
+      <c r="X18" t="n">
+        <v>17.46716381549358</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1354,13 +1784,36 @@
       </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>52.5698</t>
+          <t>52.5588</t>
         </is>
       </c>
       <c r="N19" t="inlineStr"/>
       <c r="O19" t="inlineStr"/>
       <c r="P19" t="inlineStr"/>
       <c r="Q19" t="inlineStr"/>
+      <c r="R19" t="inlineStr">
+        <is>
+          <t>48.9568</t>
+        </is>
+      </c>
+      <c r="S19" t="n">
+        <v>41</v>
+      </c>
+      <c r="T19" t="n">
+        <v>19</v>
+      </c>
+      <c r="U19" t="n">
+        <v>29.30702023417723</v>
+      </c>
+      <c r="V19" t="n">
+        <v>2</v>
+      </c>
+      <c r="W19" t="n">
+        <v>8</v>
+      </c>
+      <c r="X19" t="n">
+        <v>17.46670349646909</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1401,13 +1854,36 @@
       </c>
       <c r="M20" t="inlineStr">
         <is>
-          <t>52.5588</t>
+          <t>52.5648</t>
         </is>
       </c>
       <c r="N20" t="inlineStr"/>
       <c r="O20" t="inlineStr"/>
       <c r="P20" t="inlineStr"/>
       <c r="Q20" t="inlineStr"/>
+      <c r="R20" t="inlineStr">
+        <is>
+          <t>48.9568</t>
+        </is>
+      </c>
+      <c r="S20" t="n">
+        <v>41</v>
+      </c>
+      <c r="T20" t="n">
+        <v>19</v>
+      </c>
+      <c r="U20" t="n">
+        <v>29.30747578263379</v>
+      </c>
+      <c r="V20" t="n">
+        <v>2</v>
+      </c>
+      <c r="W20" t="n">
+        <v>8</v>
+      </c>
+      <c r="X20" t="n">
+        <v>17.46691257702675</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1448,13 +1924,36 @@
       </c>
       <c r="M21" t="inlineStr">
         <is>
-          <t>52.5648</t>
+          <t>52.5718</t>
         </is>
       </c>
       <c r="N21" t="inlineStr"/>
       <c r="O21" t="inlineStr"/>
       <c r="P21" t="inlineStr"/>
       <c r="Q21" t="inlineStr"/>
+      <c r="R21" t="inlineStr">
+        <is>
+          <t>48.9568</t>
+        </is>
+      </c>
+      <c r="S21" t="n">
+        <v>41</v>
+      </c>
+      <c r="T21" t="n">
+        <v>19</v>
+      </c>
+      <c r="U21" t="n">
+        <v>29.30763758129785</v>
+      </c>
+      <c r="V21" t="n">
+        <v>2</v>
+      </c>
+      <c r="W21" t="n">
+        <v>8</v>
+      </c>
+      <c r="X21" t="n">
+        <v>17.46686742840751</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>